<commit_message>
final version, as of 15.7.15
</commit_message>
<xml_diff>
--- a/Output/VGL GPUs.xlsx
+++ b/Output/VGL GPUs.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Documents\Bachelorarbeit code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Documents\Bachelorarbeit\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>MAC Cluster</t>
   </si>
@@ -109,6 +109,12 @@
   <si>
     <t>Partially Resident Textures</t>
   </si>
+  <si>
+    <t>Xeon</t>
+  </si>
+  <si>
+    <t>Phenom II x6</t>
+  </si>
 </sst>
 </file>
 
@@ -134,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -342,19 +348,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -387,6 +435,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -447,7 +518,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -528,11 +599,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-521192320"/>
-        <c:axId val="-521198848"/>
+        <c:axId val="-1535231648"/>
+        <c:axId val="-1535235456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-521192320"/>
+        <c:axId val="-1535231648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,10 +643,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-521198848"/>
+        <c:crossAx val="-1535235456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -583,7 +654,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-521198848"/>
+        <c:axId val="-1535235456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,10 +702,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-521192320"/>
+        <c:crossAx val="-1535231648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="100"/>
@@ -673,7 +744,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -725,7 +796,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -784,13 +855,13 @@
                 <c:formatCode>#.##0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.226</c:v>
+                  <c:v>3226</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.331</c:v>
+                  <c:v>1331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.488</c:v>
+                  <c:v>1488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,11 +877,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-521193952"/>
-        <c:axId val="-633149312"/>
+        <c:axId val="-1535224576"/>
+        <c:axId val="-1535224032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-521193952"/>
+        <c:axId val="-1535224576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,10 +921,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-633149312"/>
+        <c:crossAx val="-1535224032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -861,7 +932,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-633149312"/>
+        <c:axId val="-1535224032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,10 +980,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-521193952"/>
+        <c:crossAx val="-1535224576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -951,7 +1022,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1003,7 +1074,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1084,11 +1155,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-326430752"/>
-        <c:axId val="-326431840"/>
+        <c:axId val="-1535217504"/>
+        <c:axId val="-1535216960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-326430752"/>
+        <c:axId val="-1535217504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,10 +1199,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326431840"/>
+        <c:crossAx val="-1535216960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1139,7 +1210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-326431840"/>
+        <c:axId val="-1535216960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,10 +1258,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326430752"/>
+        <c:crossAx val="-1535217504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1228,7 +1299,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1280,7 +1351,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1361,11 +1432,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-326430208"/>
-        <c:axId val="-326434560"/>
+        <c:axId val="-1535216416"/>
+        <c:axId val="-1535208800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-326430208"/>
+        <c:axId val="-1535216416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1405,10 +1476,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326434560"/>
+        <c:crossAx val="-1535208800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1416,7 +1487,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-326434560"/>
+        <c:axId val="-1535208800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,10 +1535,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326430208"/>
+        <c:crossAx val="-1535216416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1505,7 +1576,543 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Tahiti</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tesla</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Barts</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Xeon</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Phenom II x6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>#.##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3226</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1488</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>332.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55.55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="-1535215328"/>
+        <c:axId val="-1535214240"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent1">
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent1">
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent1">
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$B$4:$F$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>Tahiti</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Tesla</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Barts</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Xeon</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Phenom II x6</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$B$5:$F$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>900</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>650</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>775</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:gradFill rotWithShape="1">
+                    <a:gsLst>
+                      <a:gs pos="0">
+                        <a:schemeClr val="accent2">
+                          <a:satMod val="103000"/>
+                          <a:lumMod val="102000"/>
+                          <a:tint val="94000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="50000">
+                        <a:schemeClr val="accent2">
+                          <a:satMod val="110000"/>
+                          <a:lumMod val="100000"/>
+                          <a:shade val="100000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                      <a:gs pos="100000">
+                        <a:schemeClr val="accent2">
+                          <a:lumMod val="99000"/>
+                          <a:satMod val="120000"/>
+                          <a:shade val="78000"/>
+                        </a:schemeClr>
+                      </a:gs>
+                    </a:gsLst>
+                    <a:lin ang="5400000" scaled="0"/>
+                  </a:gradFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$B$4:$F$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>Tahiti</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Tesla</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Barts</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Xeon</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Phenom II x6</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Tabelle1!$B$6:$F$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>28</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1535215328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1535214240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1535214240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>GFLOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1535215328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1676,6 +2283,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3688,17 +4335,513 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>197069</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>131380</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>74230</xdr:rowOff>
@@ -3722,13 +4865,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>210207</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>70287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>144518</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>177362</xdr:rowOff>
@@ -3752,13 +4895,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>144517</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>98535</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>59120</xdr:rowOff>
@@ -3782,13 +4925,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>157656</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>63719</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>98535</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>183931</xdr:rowOff>
@@ -3805,6 +4948,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1139686</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>59635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>92766</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4076,197 +5249,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>900</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>650</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>775</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>28</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>16</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>12</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12">
-        <v>3.226</v>
+      <c r="B7" s="10">
+        <v>3226</v>
       </c>
-      <c r="C7" s="12">
-        <v>1.331</v>
+      <c r="C7" s="10">
+        <v>1331</v>
       </c>
-      <c r="D7" s="12">
-        <v>1.488</v>
+      <c r="D7" s="10">
+        <v>1488</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="24">
+        <v>332.8</v>
+      </c>
+      <c r="F7" s="24">
+        <v>55.55</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>4096</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>6144</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>1024</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>176</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>178</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>128</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <v>806</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="14">
         <v>665</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>